<commit_message>
Confusion matrix and image
</commit_message>
<xml_diff>
--- a/Assignment2Results.xlsx
+++ b/Assignment2Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sajidkhan/Desktop/ML/Assignment2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{03FAC7FA-C9C8-B348-8D5A-63239CC82C16}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{E29BE751-571A-124E-B025-782EE44FADB4}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11520" yWindow="460" windowWidth="17280" windowHeight="16120" activeTab="2" xr2:uid="{A4153FB4-58E5-CC4E-975F-A3FEDF3DBED8}"/>
   </bookViews>
@@ -1902,7 +1902,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1927,7 +1927,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>6.9</v>
+        <v>10.1</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -1938,7 +1938,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>9.1999999999999993</v>
+        <v>10.9</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -1949,7 +1949,7 @@
         <v>100</v>
       </c>
       <c r="B4">
-        <v>65.2</v>
+        <v>69.8</v>
       </c>
       <c r="C4">
         <v>5</v>
@@ -1960,10 +1960,10 @@
         <v>1000</v>
       </c>
       <c r="B5">
-        <v>92.4</v>
+        <v>93.2</v>
       </c>
       <c r="C5">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -1971,10 +1971,10 @@
         <v>10000</v>
       </c>
       <c r="B6">
-        <v>98.8</v>
+        <v>98.7</v>
       </c>
       <c r="C6">
-        <v>465</v>
+        <v>429</v>
       </c>
     </row>
   </sheetData>

</xml_diff>